<commit_message>
Updated talks and talk map
</commit_message>
<xml_diff>
--- a/markdown_generator/talks.xlsx
+++ b/markdown_generator/talks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33120" yWindow="-3660" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-30100" yWindow="-3620" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>title</t>
   </si>
@@ -111,6 +111,81 @@
   </si>
   <si>
     <t>2017-09-09</t>
+  </si>
+  <si>
+    <t>LIGO Detector Characterization Update</t>
+  </si>
+  <si>
+    <t>2016-03-17</t>
+  </si>
+  <si>
+    <t>Pasadena, CA</t>
+  </si>
+  <si>
+    <t>Plenary talk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burst Data Quality </t>
+  </si>
+  <si>
+    <t>2015-09-03</t>
+  </si>
+  <si>
+    <t>Budapest, Hungary</t>
+  </si>
+  <si>
+    <t>Introduction to Advanced LIGO Burst Data Quality</t>
+  </si>
+  <si>
+    <t>Albert Einstein Institute</t>
+  </si>
+  <si>
+    <t>Hannover, Germany</t>
+  </si>
+  <si>
+    <t>seminar</t>
+  </si>
+  <si>
+    <t>Cardiff University</t>
+  </si>
+  <si>
+    <t>Cardiff, Wales</t>
+  </si>
+  <si>
+    <t>2015-08-25</t>
+  </si>
+  <si>
+    <t>2015-08-18</t>
+  </si>
+  <si>
+    <t>Characterization of the Instrumental Background of Advanced LIGO's Gravitational Wave Burst Search</t>
+  </si>
+  <si>
+    <t>GCG</t>
+  </si>
+  <si>
+    <t>Gulf Coast Gravity Meeting</t>
+  </si>
+  <si>
+    <t>2015-02-15</t>
+  </si>
+  <si>
+    <t>Gainesville, FL</t>
+  </si>
+  <si>
+    <t>Burst Data Quality in Livingston Full Interferometer</t>
+  </si>
+  <si>
+    <t>2014-08-15</t>
+  </si>
+  <si>
+    <t>Stanford, CA</t>
+  </si>
+  <si>
+    <t>Update on Ongoing Projects in Advanced LIGO Suspensions Detector Characterization</t>
+  </si>
+  <si>
+    <t>2013-09-17</t>
   </si>
 </sst>
 </file>
@@ -440,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,6 +624,128 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>